<commit_message>
Update: Menu.xlsx File from Crowdin
</commit_message>
<xml_diff>
--- a/ja/Menu.xlsx
+++ b/ja/Menu.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F554BD2B-745B-4B97-998E-76F9031BDA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Main" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="534">
   <si>
     <t>日本語</t>
   </si>
@@ -918,34 +914,34 @@
     <t>LanguageSelectItemDesc</t>
   </si>
   <si>
-    <t>使用する~b~言語~s~を変更します。
+    <t xml:space="preserve">使用する~b~言語~s~を変更します。
 これは~g~DekoKiyo作のプラグインのみ~s~に適用されます。</t>
   </si>
   <si>
-    <t>Change ~b~Language~s~ to use.
+    <t xml:space="preserve">Change ~b~Language~s~ to use.
 This only applies to ~g~plugins created by DekoKiyo~s~.</t>
   </si>
   <si>
-    <t>~b~Sprache~s~ ändern.
+    <t xml:space="preserve">~b~Sprache~s~ ändern.
 Diese Option funktioniert nur für ~g~plugins von DekoKiyo~s~.</t>
   </si>
   <si>
-    <t>Cambia ~b~Lingua~s~ da usare.
+    <t xml:space="preserve">Cambia ~b~Lingua~s~ da usare.
 Questo vale solo per ~g~plugin creati da DekoKiyo~s~</t>
   </si>
   <si>
     <t>Mude o ~o~Idioma do~s~'s ~b~DynamicLSPDFR~s~.</t>
   </si>
   <si>
-    <t>Kullanmak istediğin ~b~dili~s~ seç.
+    <t xml:space="preserve">Kullanmak istediğin ~b~dili~s~ seç.
 Sadece ~g~DekoKiyo'nun eklentilerini kapsar~s~.</t>
   </si>
   <si>
-    <t>Zmente ~b~Jazyk~s~ ktery chcete pouzivat.
+    <t xml:space="preserve">Zmente ~b~Jazyk~s~ ktery chcete pouzivat.
 To plati pouze pro ~g~pluginy vytvorene DekoKiyo~s~.</t>
   </si>
   <si>
-    <t>Pakeisti naudojamą ~b~kalbą~s~
+    <t xml:space="preserve">Pakeisti naudojamą ~b~kalbą~s~
 Tai taikoma tik ~g~DekoKiyo modifikacijom~s~</t>
   </si>
   <si>
@@ -1036,15 +1032,15 @@
     <t>PylonFreezeItemDesc</t>
   </si>
   <si>
-    <t>有効だと~o~パイロン~s~が設置された場所に固定されます。
+    <t xml:space="preserve">有効だと~o~パイロン~s~が設置された場所に固定されます。
 固定されていない場合、当たると動いたり、倒れます。</t>
   </si>
   <si>
-    <t>啓動時，  ~o~ 三角錐 ~s~ 將會被固定，無法被撞擊
+    <t xml:space="preserve">啓動時，  ~o~ 三角錐 ~s~ 將會被固定，無法被撞擊
 如未啓動，三角錐遭到撞擊時將會被撞倒。</t>
   </si>
   <si>
-    <t>When enabled, the ~o~pylon ~s~ will be anchored to where it was placed.
+    <t xml:space="preserve">When enabled, the ~o~pylon ~s~ will be anchored to where it was placed.
 If it's not enabled, it will move or fall when hit.</t>
   </si>
   <si>
@@ -1052,38 +1048,38 @@
 Falls diese Funktion ~o~nicht~s~ aktiviert ist, wird der Pylon umfallen. </t>
   </si>
   <si>
-    <t>Quando abilitato, il cono sarà ancorato al punto in cui è stato posizionato.
+    <t xml:space="preserve">Quando abilitato, il cono sarà ancorato al punto in cui è stato posizionato.
  Se non è abilitato, si muoverà o cadrà quando viene colpito.</t>
   </si>
   <si>
-    <t>Po włączeniu, ~o~pachołek ~s~ będzie zakotwiczony w miejscu, w którym został umieszczony.
+    <t xml:space="preserve">Po włączeniu, ~o~pachołek ~s~ będzie zakotwiczony w miejscu, w którym został umieszczony.
 Jeśli ta opcja nie jest włączona, będzie się poruszał lub spadnie kiedy uderzony.</t>
   </si>
   <si>
-    <t>Quando habilitados, os ~o~cones ~s~ ficarão grudados nos lugares em que foram postos.
+    <t xml:space="preserve">Quando habilitados, os ~o~cones ~s~ ficarão grudados nos lugares em que foram postos.
 Quando não está habilitado, os cones se moverão e cairão quando atingidos.</t>
   </si>
   <si>
-    <t>Когда этот параметр включен, ~o~конус ~s~ будет закреплен на том месте, где он был установлен.
+    <t xml:space="preserve">Когда этот параметр включен, ~o~конус ~s~ будет закреплен на том месте, где он был установлен.
 Если он не включен, то при ударе он сдвинется или упадет.</t>
   </si>
   <si>
-    <t>Cuando está habilitado, ~o~pilones~s~ se anclará a la ubicación donde se colocó.
+    <t xml:space="preserve">Cuando está habilitado, ~o~pilones~s~ se anclará a la ubicación donde se colocó.
 Si no está habilitado, se moverá o caerá cuando sea golpeado.</t>
   </si>
   <si>
-    <t>Bu özelliği aktifleştirirseniz, ~o~dubalar~s~ devrilmez.
+    <t xml:space="preserve">Bu özelliği aktifleştirirseniz, ~o~dubalar~s~ devrilmez.
 Eğer devre dışı bırakırsanız, çarptığınızda devrilir.</t>
   </si>
   <si>
     <t>Pokud tohle neni, ~o~povoleno ~s~ tak NPC mohou je schodit ci prejet.</t>
   </si>
   <si>
-    <t>När denna är aktiverad, kommer ~o~konen ~s~ bli fast satt där den placeras.
+    <t xml:space="preserve">När denna är aktiverad, kommer ~o~konen ~s~ bli fast satt där den placeras.
 Om denna inte är aktiverad kommer konen kunna ramla och flyttas.</t>
   </si>
   <si>
-    <t>Kai įjungta, ~o~kūgiai~s~ sustings savo vietoje..
+    <t xml:space="preserve">Kai įjungta, ~o~kūgiai~s~ sustings savo vietoje..
 Jeigu jie nėra sustingdinti, jie galės laisvai pervirsti, nukristi.</t>
   </si>
   <si>
@@ -1132,91 +1128,91 @@
     <t>SetPylonPosesDesc</t>
   </si>
   <si>
-    <t>~o~パイロン~s~の設置位置を指定します。
+    <t xml:space="preserve">~o~パイロン~s~の設置位置を指定します。
 タブの背景で状態を示しています。
 ~y~黄色~s~: 未指定
 ~g~緑色~s~: 指定済み
 ~r~赤色~s~: 指定中</t>
   </si>
   <si>
-    <t>指定 ~o~ 三角錐 ~s~ 的位置。
+    <t xml:space="preserve">指定 ~o~ 三角錐 ~s~ 的位置。
 選項卡的背景指示狀態。（此句翻譯將會於下次更新時予以修正）
 ~y~ 黃色 ~s~: 無
 ~g~ 綠色 ~s~: 被選擇
 ~r~ 紅色 ~s~: 選擇中</t>
   </si>
   <si>
-    <t>Specifies the place positions of the ~o~pylons~s~.
+    <t xml:space="preserve">Specifies the place positions of the ~o~pylons~s~.
 The background of the tab indicates the state.
 ~y~Yellow ~s~: None
 ~g~Green ~s~: Specified
 ~r~Red ~s~: Specifying now</t>
   </si>
   <si>
-    <t>Wählt die Position der ~o~Pylonen~s~ aus.
+    <t xml:space="preserve">Wählt die Position der ~o~Pylonen~s~ aus.
 Die Hintergrundanzeige zeigt den Zustand.
 ~y~Yellow ~s~: Keine
 ~g~Green ~s~: Ausgewählt
 ~r~Red ~s~: Wird ausgewählt</t>
   </si>
   <si>
-    <t>Specifica la posizione dei coni stradale.
+    <t xml:space="preserve">Specifica la posizione dei coni stradale.
  Lo sfondo della scheda indica lo stato.
  ~y~Giallo ~s~: nessuno
  ~g~Verde ~s~: specificato
  ~r~Rosso ~s~: Specificato ora</t>
   </si>
   <si>
-    <t>Podaje pozycję ~o~pachołków~s~.
+    <t xml:space="preserve">Podaje pozycję ~o~pachołków~s~.
 Kolor zakładki oznacza stan:
 ~y~Żółty ~s~: Żaden
 ~g~Zielony ~s~: Określony
 ~r~Czerwony ~s~: Określany</t>
   </si>
   <si>
-    <t>Especifica a posição dos ~o~cones~s~.
+    <t xml:space="preserve">Especifica a posição dos ~o~cones~s~.
 A cor fundo indica o estado.
 ~y~Amarelo ~s~: Nenhum
 ~g~Verde ~s~: Especificado
 ~r~Vermelho ~s~: Especificando agora</t>
   </si>
   <si>
-    <t>Определяет расположение ~o~конусов~s~.
+    <t xml:space="preserve">Определяет расположение ~o~конусов~s~.
 Фон вкладки указывает на состояние.
 ~y~ Желтый ~s~: Отсутствует
 ~g~Зеленый ~s~: Указано
 ~r~Красный ~s~: Уточняем сейчас</t>
   </si>
   <si>
-    <t>Especifica las posiciones del lugar de los ~o~pilones~s~.
+    <t xml:space="preserve">Especifica las posiciones del lugar de los ~o~pilones~s~.
 Color indica estado de los pilones.
 ~y~Amarillo~s~: Ninguno
 ~g~Verde~s~: Especificado
 ~r~Rojo~s~: Especificando ahora</t>
   </si>
   <si>
-    <t>~o~Dubaların~s~ konumunu belirler.
+    <t xml:space="preserve">~o~Dubaların~s~ konumunu belirler.
 Durumun arka plandaki işlemlerini gösterir.
 ~y~Sarı ~s~: Boş
 ~g~Yeşil ~s~: Belirtilmiş
 ~r~Kırmızı ~s~: Belirleniyor</t>
   </si>
   <si>
-    <t>Urcuje umisteni ~o~dopravnich kuzelu~s~.
+    <t xml:space="preserve">Urcuje umisteni ~o~dopravnich kuzelu~s~.
 Pozadi menu oznacuje stav.
 ~y~Zluta ~s~: Zadny
 ~g~Zelena ~s~: Urceno
 ~r~Cervena ~s~: Specifikuje se nyni</t>
   </si>
   <si>
-    <t>Anger platspositionerna för ~o~konerna~s~.
+    <t xml:space="preserve">Anger platspositionerna för ~o~konerna~s~.
 Bakgrundsfärgen indikerar tillståndet.
 ~y~Gul ~s~: Inga
 ~g~Grön ~s~: Specificerad
 ~r~Röd ~s~: Specificerar nu</t>
   </si>
   <si>
-    <t>Nustato ~o~kūgių~s~ dėliojimo vietą
+    <t xml:space="preserve">Nustato ~o~kūgių~s~ dėliojimo vietą
 Fonas nurodo nustatymo statusą.
 ~y~Geltona~s~: Joksai
 ~g~Žalia~s~: Nustatyta
@@ -1226,55 +1222,55 @@
     <t>PylonCountItemDesc</t>
   </si>
   <si>
-    <t>~o~パイロン~s~の設置本数を指定します。
+    <t xml:space="preserve">~o~パイロン~s~の設置本数を指定します。
 現在の本数: {0}</t>
   </si>
   <si>
-    <t>一組 ~o~ 三角錐 ~s~ 的數量
+    <t xml:space="preserve">一組 ~o~ 三角錐 ~s~ 的數量
 目前數量: {0}</t>
   </si>
   <si>
-    <t>Set for ~o~pylons~s~ count.
+    <t xml:space="preserve">Set for ~o~pylons~s~ count.
 Now count: {0}</t>
   </si>
   <si>
-    <t>Gibt die aktuelle Anzahl von platzierten Pylonen an.
+    <t xml:space="preserve">Gibt die aktuelle Anzahl von platzierten Pylonen an.
 Anzahl an Pylonen: {0}</t>
   </si>
   <si>
-    <t>Impostato per il conteggio di cono stradale
+    <t xml:space="preserve">Impostato per il conteggio di cono stradale
  Ora conta: {0}</t>
   </si>
   <si>
-    <t>Ilość ~o~pachołków~s~
+    <t xml:space="preserve">Ilość ~o~pachołków~s~
 Obecna ilość: {0}</t>
   </si>
   <si>
-    <t>Defina a quantidade de ~o~cones~s~.
+    <t xml:space="preserve">Defina a quantidade de ~o~cones~s~.
 Quantidade atual: {0}</t>
   </si>
   <si>
-    <t>Установлено для ~o~ количества конусов~s~.
+    <t xml:space="preserve">Установлено для ~o~ количества конусов~s~.
 Теперь посчитайте: {0}</t>
   </si>
   <si>
-    <t>Cantidad de los ~o~pilones~s~.
+    <t xml:space="preserve">Cantidad de los ~o~pilones~s~.
 Cantidad ahora: {0}</t>
   </si>
   <si>
-    <t>~o~Dubalar~s~ için adet belirleyin.
+    <t xml:space="preserve">~o~Dubalar~s~ için adet belirleyin.
 Şuanki adet: {0}</t>
   </si>
   <si>
-    <t>Nastavte na pocet ~o~dopravnich kuzelu~s~.
+    <t xml:space="preserve">Nastavte na pocet ~o~dopravnich kuzelu~s~.
 Nyni pocitejte: {0}</t>
   </si>
   <si>
-    <t>Anger antalet ~o~koner ~s~ som ska sättas ut.
+    <t xml:space="preserve">Anger antalet ~o~koner ~s~ som ska sättas ut.
 Nuvarande antal: {0}</t>
   </si>
   <si>
-    <t>Nustatyti ~o~kūgių~s~ kiekį
+    <t xml:space="preserve">Nustatyti ~o~kūgių~s~ kiekį
 Dabartinis: {0}</t>
   </si>
   <si>
@@ -1323,55 +1319,55 @@
     <t>ResetPylonItemDesc</t>
   </si>
   <si>
-    <t>~o~パイロン~s~の設定を~r~リセット~s~します。
+    <t xml:space="preserve">~o~パイロン~s~の設定を~r~リセット~s~します。
 (既存のパイロンは~y~削除されません~s~。)</t>
   </si>
   <si>
-    <t>~r~ 重置 ~s~ ~o~ 三角錐 ~s~ 的設定。
+    <t xml:space="preserve">~r~ 重置 ~s~ ~o~ 三角錐 ~s~ 的設定。
 ( ~y~ 不會取消 ~s~ 多出之三角錐)。</t>
   </si>
   <si>
-    <t>~r~Reset~s~ ~o~pylon~s~ settings.
+    <t xml:space="preserve">~r~Reset~s~ ~o~pylon~s~ settings.
 (~y~No delete~s~ existing pylons.)</t>
   </si>
   <si>
-    <t>Setzt die Pylonen-Einstellungen zurück.
+    <t xml:space="preserve">Setzt die Pylonen-Einstellungen zurück.
  Bestehende Pylonen werden bei diesem Prozess ~y~nicht~s~ gelöscht.</t>
   </si>
   <si>
-    <t>Ripristina le impostazioni del cono.
+    <t xml:space="preserve">Ripristina le impostazioni del cono.
  Nessuna eliminazione dei coni esistenti.</t>
   </si>
   <si>
-    <t>~r~Resetuj~s~ ustawienia ~o~pachołków~s~
+    <t xml:space="preserve">~r~Resetuj~s~ ustawienia ~o~pachołków~s~
 (~y~Nie usuwa~s~ istniejących pachołków.)</t>
   </si>
   <si>
-    <t>~r~Redefine~s~ as configurações do ~o~cone~s~
+    <t xml:space="preserve">~r~Redefine~s~ as configurações do ~o~cone~s~
 (~y~Não apaga~s~ cones que já existem.)</t>
   </si>
   <si>
-    <t>~r ~Сбросьте~s ~ ~o~настройки конусов ~s~.
+    <t xml:space="preserve">~r ~Сбросьте~s ~ ~o~настройки конусов ~s~.
 (~y~Не удалять~s~ существующие конусные знаки.)</t>
   </si>
   <si>
-    <t>~r~Reiniciar~s~ ajustes de los ~o~pilones~s~.
+    <t xml:space="preserve">~r~Reiniciar~s~ ajustes de los ~o~pilones~s~.
 (~y~Esto no elimina~s~ los pilones existentes.)</t>
   </si>
   <si>
-    <t>~o~Dubaların~s~ ayarlarını ~r~sıfırlar~s~.
+    <t xml:space="preserve">~o~Dubaların~s~ ayarlarını ~r~sıfırlar~s~.
 (Mevcut dubaları ~y~silmez~s~.)</t>
   </si>
   <si>
-    <t>~r~Odstranis~s~ ~o~prave pokladane~s~ dopravni kuzele.
+    <t xml:space="preserve">~r~Odstranis~s~ ~o~prave pokladane~s~ dopravni kuzele.
 (~y~Zadne odstraneni~s~ existujicich dopravnich kuzelu.)</t>
   </si>
   <si>
-    <t>~r~Återställ~s~ ~o~kon~s~ inställningar.
+    <t xml:space="preserve">~r~Återställ~s~ ~o~kon~s~ inställningar.
 (Befintliga koner ~y~raderas ej~s~.)</t>
   </si>
   <si>
-    <t>~r~Perrinkti~s~ ~o~kūgių~s~ nustatymus
+    <t xml:space="preserve">~r~Perrinkti~s~ ~o~kūgių~s~ nustatymus
 (~y~Neištrina~s~ esančių kūgių)</t>
   </si>
   <si>
@@ -1501,122 +1497,122 @@
     <t>LanguageMenuDesc</t>
   </si>
   <si>
-    <t>変更したい~b~言語~s~を選択してください。
+    <t xml:space="preserve">変更したい~b~言語~s~を選択してください。
 ~g~カスタム翻訳~s~は~o~「Custom」~s~を選択してください。</t>
   </si>
   <si>
-    <t>請選擇你需要的 ~b~ 語言 ~s~ 。
+    <t xml:space="preserve">請選擇你需要的 ~b~ 語言 ~s~ 。
 如果你希望使用 ~g~ 自行編譯的翻譯 ~s~ , 請選擇 ~o~ "Custom" ~s~ 。</t>
   </si>
   <si>
-    <t>Select ~b~the Language~s~ which you want.
+    <t xml:space="preserve">Select ~b~the Language~s~ which you want.
 If you want to change ~g~Custom Translation~s~, please select ~o~"Custom"~s~.</t>
   </si>
   <si>
-    <t>Wähle ~b~die Sprache~s~ die du möchtest.
+    <t xml:space="preserve">Wähle ~b~die Sprache~s~ die du möchtest.
 Falls du ~g~Zufalls Übersetzung~s~, bitte wähle ~o~"Custom''~s~ aus.</t>
   </si>
   <si>
     <t>Lingua Menù</t>
   </si>
   <si>
-    <t>Wybierz ~b~język~s~, którego chcesz używać.
+    <t xml:space="preserve">Wybierz ~b~język~s~, którego chcesz używać.
 Jeżeli chcesz zmienić ~g~niestandardowe tłumaczenie~s~, proszę wybierz ~o~"Niestandardowe"~s.</t>
   </si>
   <si>
-    <t>Escolha ~b~o idioma~s~ que você quer.
+    <t xml:space="preserve">Escolha ~b~o idioma~s~ que você quer.
 Se você quer mudar para ~g~Traduções customizadas~s~, selecione ~o~"Customizado"~s~.</t>
   </si>
   <si>
     <t>Описание языкового меню</t>
   </si>
   <si>
-    <t>Elegir ~b~el idioma~s~, que quieres usar.
+    <t xml:space="preserve">Elegir ~b~el idioma~s~, que quieres usar.
 Si quieres cambiar ~g~traducción personalizada~s~, elige ~o~"personalizada"~s.</t>
   </si>
   <si>
     <t>~g~Kullanmak istediğin dili~s~ seç.</t>
   </si>
   <si>
-    <t>Vyberte ~b~jazyk~s~, který chcete.
+    <t xml:space="preserve">Vyberte ~b~jazyk~s~, který chcete.
 Chcete-li zmenit ~g~Vlastní preklad~s~, vyberte ~na~"Vlastní"~s~.</t>
   </si>
   <si>
-    <t>Vælg ~b~Sproget~s~ du vil bruge.
+    <t xml:space="preserve">Vælg ~b~Sproget~s~ du vil bruge.
 Hvis du gerne vil bruge ~g~Brugerdefineret Oversættelse~s~, vælg venligst ~o~"Custom"~s~.</t>
   </si>
   <si>
-    <t>Välj  ~b~språket~s~ du vill ha.
+    <t xml:space="preserve">Välj  ~b~språket~s~ du vill ha.
 Om du vill ändra ~g~Anpassad Översättning~s~, Välj ~o~"Anpassad"~s~.</t>
   </si>
   <si>
-    <t>Valitse ~b~Kieli~s~ Jonka haluat.
+    <t xml:space="preserve">Valitse ~b~Kieli~s~ Jonka haluat.
 Jos haluat vaihtaa ~g~Mukautettu käännös~s~, valitse ~o~"Mukautettu"~s~.</t>
   </si>
   <si>
-    <t>Pasirinkite ~b~kalbą~s~ kurią norite naudoti..
+    <t xml:space="preserve">Pasirinkite ~b~kalbą~s~ kurią norite naudoti..
 Jeigu norite pakeisti ~g~atskirą vertimą~s~, prašome pasirinkti ~o~"Atskiras"~s~.</t>
   </si>
   <si>
     <t>CustomLanguageMenuDesc</t>
   </si>
   <si>
-    <t>~h~~y~【注意】~s~~h~
+    <t xml:space="preserve">~h~~y~【注意】~s~~h~
 ~r~割り当てられていないキーの翻訳には自動的に英語翻訳が適用されます。~s~</t>
   </si>
   <si>
-    <t>~h~~y~ 【注意】 ~s~~h~
+    <t xml:space="preserve">~h~~y~ 【注意】 ~s~~h~
 ~r~ 尚未翻譯之詞語會自動使用英語之翻譯。 ~s~</t>
   </si>
   <si>
-    <t>~h~~y~ATTENTION~s~~h~
+    <t xml:space="preserve">~h~~y~ATTENTION~s~~h~
 ~r~The key which has no translate will assign  English Translation automatically.~s~</t>
   </si>
   <si>
-    <t>~h~~y~ATTENTION~s~~h~
+    <t xml:space="preserve">~h~~y~ATTENTION~s~~h~
 ~r~Wörter die noch nicht von unserem Übersetzungs-Team übersetzt worden sind, werden automatisch durch die englischen Wörter ersetzt.~s~</t>
   </si>
   <si>
     <t xml:space="preserve">Lingua personalizzata Menu </t>
   </si>
   <si>
-    <t>~h~~y~UWAGA~s~~h~
+    <t xml:space="preserve">~h~~y~UWAGA~s~~h~
 ~r~Wyrazy bez gotowego tłumaczenia bedą automatycznie używać słów angielskich.~s~</t>
   </si>
   <si>
-    <t>~h~~y~ATENÇÃO~s~~h~
+    <t xml:space="preserve">~h~~y~ATENÇÃO~s~~h~
 ~r~As palavras que não foram traduzidas serão automaticamente mudadas para o Inglês.~s~</t>
   </si>
   <si>
-    <t>~h~~y~ВНИМАНИЕ~s~~h~
+    <t xml:space="preserve">~h~~y~ВНИМАНИЕ~s~~h~
 ~r~ Клавиша, у которой нет перевода, автоматически назначит перевод на английский.~s~</t>
   </si>
   <si>
-    <t>~h~~y~ ATENCIÓN ~s~~h~
+    <t xml:space="preserve">~h~~y~ ATENCIÓN ~s~~h~
 ~r~Palabras que no tienen traducción, usarán la traducción al ingles~s~</t>
   </si>
   <si>
-    <t>~h~~y~DİKKAT~s~~h~
+    <t xml:space="preserve">~h~~y~DİKKAT~s~~h~
 ~r~Çevirilmeyen satırlar otomatik olarak İngilizce ayarlanır.~s~</t>
   </si>
   <si>
-    <t>~h~~y~POZOR~s~~h~
+    <t xml:space="preserve">~h~~y~POZOR~s~~h~
 ~r~Custom, se dava automaticky do anglickeho prekladu. Pokud vy si ho sami neupravite.~s~</t>
   </si>
   <si>
-    <t>~h~~y~ADVARNING~s~~h~
+    <t xml:space="preserve">~h~~y~ADVARNING~s~~h~
 ~r~Nøglen har ingen oversættelse, vil automatisk tildele engelsk oversættelse.~s~</t>
   </si>
   <si>
-    <t>~h~~y~VARNING~s~~h~
+    <t xml:space="preserve">~h~~y~VARNING~s~~h~
 ~r~Orden som inte har någon översättning får engelsk översättning automatiskt.~s~</t>
   </si>
   <si>
-    <t>~h~~y~HUOMIO~s~~h~
+    <t xml:space="preserve">~h~~y~HUOMIO~s~~h~
 ~r~Avain, jolla ei ole käännöstä, määrittää englanninkielisen käännöksen automaattisesti.~s~</t>
   </si>
   <si>
-    <t>~h~~y~DĖMĖSIO~s~~h~
+    <t xml:space="preserve">~h~~y~DĖMĖSIO~s~~h~
 ~r~Šis klavišas kuris neturi vertimo priskirs Anglišką vertimą automatiškai.~s~</t>
   </si>
   <si>
@@ -1741,38 +1737,26 @@
   </si>
   <si>
     <t>Vertimo raida: {0}</t>
-  </si>
-  <si>
-    <t>Change ~b~Language~s~ to use.
-This only applies to ~g~plugins created by DekoKiyo~s~.</t>
-    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <charset val="128"/>
+      <color theme="1"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1806,7 +1790,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2142,20 +2126,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
     <col min="2" max="22" width="30.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2221,7 +2200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -2279,7 +2258,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -2331,7 +2310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -2385,7 +2364,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
@@ -2437,7 +2416,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
@@ -2489,7 +2468,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
@@ -2541,7 +2520,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>108</v>
       </c>
@@ -2593,7 +2572,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -2645,7 +2624,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>136</v>
       </c>
@@ -2697,7 +2676,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>150</v>
       </c>
@@ -2749,7 +2728,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -2801,7 +2780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>171</v>
       </c>
@@ -2853,7 +2832,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>185</v>
       </c>
@@ -2905,7 +2884,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>199</v>
       </c>
@@ -2957,7 +2936,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>213</v>
       </c>
@@ -3009,7 +2988,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>227</v>
       </c>
@@ -3061,7 +3040,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>241</v>
       </c>
@@ -3113,7 +3092,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" ht="13.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>255</v>
       </c>
@@ -3171,7 +3150,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>272</v>
       </c>
@@ -3227,7 +3206,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>286</v>
       </c>
@@ -3279,7 +3258,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="23" ht="40.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>299</v>
       </c>
@@ -3289,7 +3268,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="3" t="s">
-        <v>534</v>
+        <v>301</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
@@ -3321,7 +3300,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>308</v>
       </c>
@@ -3373,7 +3352,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>322</v>
       </c>
@@ -3425,7 +3404,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>336</v>
       </c>
@@ -3477,7 +3456,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>350</v>
       </c>
@@ -3529,7 +3508,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>364</v>
       </c>
@@ -3581,7 +3560,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>378</v>
       </c>
@@ -3633,7 +3612,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>392</v>
       </c>
@@ -3685,7 +3664,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>406</v>
       </c>
@@ -3737,7 +3716,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>420</v>
       </c>
@@ -3789,7 +3768,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>434</v>
       </c>
@@ -3841,7 +3820,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>448</v>
       </c>
@@ -3893,7 +3872,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" ht="67.5" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>461</v>
       </c>
@@ -3949,7 +3928,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" ht="54" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>477</v>
       </c>
@@ -4005,49 +3984,12 @@
         <v>492</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" ht="40.5" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1" t="s">
-        <v>307</v>
-      </c>
     </row>
-    <row r="38" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" ht="27" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>493</v>
       </c>
@@ -4089,7 +4031,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" ht="27" customHeight="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>502</v>
       </c>
@@ -4147,7 +4089,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>517</v>
       </c>
@@ -4206,8 +4148,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>